<commit_message>
updated building_categories input and code
</commit_message>
<xml_diff>
--- a/input/s_curves.xlsx
+++ b/input/s_curves.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Brukere-felles\lfep\EBM\task_836\Energibruksmodell\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E09BDB-5351-4A1C-82F2-9BD7F83B6042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647D420F-8128-4E3D-8CE1-0D5DF90F8E1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="16455" windowHeight="15375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="s_curve" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="24">
   <si>
-    <t>building_type</t>
-  </si>
-  <si>
     <t>average_age</t>
   </si>
   <si>
@@ -106,6 +103,9 @@
   </si>
   <si>
     <t>renovation_type</t>
+  </si>
+  <si>
+    <t>building_category</t>
   </si>
 </sst>
 </file>
@@ -509,7 +509,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
@@ -521,37 +521,37 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>4</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>5</v>
       </c>
       <c r="I1" s="9"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="7">
         <v>5</v>
@@ -574,10 +574,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1">
         <v>10</v>
@@ -600,10 +600,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="7">
         <v>60</v>
@@ -626,10 +626,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="3">
         <v>3</v>
@@ -652,10 +652,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="3">
         <v>10</v>
@@ -678,10 +678,10 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="3">
         <v>60</v>
@@ -704,10 +704,10 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="3">
         <v>3</v>
@@ -730,10 +730,10 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="3">
         <v>10</v>
@@ -756,10 +756,10 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" s="3">
         <v>50</v>
@@ -782,10 +782,10 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" s="3">
         <v>5</v>
@@ -808,10 +808,10 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" s="3">
         <v>10</v>
@@ -834,10 +834,10 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13" s="3">
         <v>50</v>
@@ -860,10 +860,10 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" s="3">
         <v>5</v>
@@ -886,10 +886,10 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" s="3">
         <v>15</v>
@@ -912,10 +912,10 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C16" s="3">
         <v>50</v>
@@ -938,10 +938,10 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17" s="3">
         <v>3</v>
@@ -964,10 +964,10 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C18" s="3">
         <v>5</v>
@@ -990,10 +990,10 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C19" s="3">
         <v>50</v>
@@ -1016,10 +1016,10 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C20" s="3">
         <v>3</v>
@@ -1042,10 +1042,10 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C21" s="3">
         <v>5</v>
@@ -1068,10 +1068,10 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C22" s="3">
         <v>50</v>
@@ -1094,10 +1094,10 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C23" s="3">
         <v>3</v>
@@ -1120,10 +1120,10 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C24" s="3">
         <v>5</v>
@@ -1146,10 +1146,10 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C25" s="3">
         <v>50</v>
@@ -1172,10 +1172,10 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C26" s="3">
         <v>3</v>
@@ -1198,10 +1198,10 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C27" s="3">
         <v>10</v>
@@ -1224,10 +1224,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C28" s="3">
         <v>50</v>
@@ -1250,10 +1250,10 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C29" s="3">
         <v>3</v>
@@ -1276,10 +1276,10 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C30" s="3">
         <v>5</v>
@@ -1302,10 +1302,10 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C31" s="3">
         <v>50</v>
@@ -1328,10 +1328,10 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C32" s="3">
         <v>3</v>
@@ -1354,10 +1354,10 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C33" s="3">
         <v>5</v>
@@ -1380,10 +1380,10 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C34" s="3">
         <v>50</v>
@@ -1406,10 +1406,10 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C35" s="3">
         <v>3</v>
@@ -1432,10 +1432,10 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C36" s="3">
         <v>15</v>
@@ -1458,10 +1458,10 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C37" s="3">
         <v>50</v>
@@ -1484,10 +1484,10 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C38" s="3">
         <v>3</v>
@@ -1510,10 +1510,10 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C39" s="3">
         <v>5</v>
@@ -1536,10 +1536,10 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C40" s="3">
         <v>50</v>

</xml_diff>